<commit_message>
cda2 & cda3 - (2)
</commit_message>
<xml_diff>
--- a/link-template.xlsx
+++ b/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60BA106-C18D-4815-82EF-AB3E30BF20A3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD710AC6-CCD6-44DB-8984-696E16E34119}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="528">
   <si>
     <t>"&gt;</t>
   </si>
@@ -1615,55 +1615,55 @@
     <t>https://aws.amazon.com/swf/faqs/</t>
   </si>
   <si>
-    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/using-cfn-describing-stacks.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://aws.amazon.com/sns/faqs/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStackResources.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://aws.amazon.com/dynamodb/faqs/</t>
-  </si>
-  <si>
-    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/parameters-section-structure.html</t>
-  </si>
-  <si>
-    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/aws-properties-ec2-instance.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-register.html </t>
-  </si>
-  <si>
-    <t>https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html#limits-secondary-indexes</t>
-  </si>
-  <si>
-    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-getatt.html</t>
-  </si>
-  <si>
     <t>http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html</t>
   </si>
   <si>
-    <t xml:space="preserve">http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_DescribeImages.html </t>
-  </si>
-  <si>
-    <t>https://aws.amazon.com/cloudformation/faqs/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://docs.aws.amazon.com/AmazonS3/latest/dev/access-policy-language-overview.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://aws.amazon.com/blogs/developer/elasticache-as-an-asp-net-session-store/ </t>
-  </si>
-  <si>
-    <t>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/SecondaryIndexes.html</t>
+    <t>https://aws.amazon.com/dynamodb/faqs/</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSSnapshots.html</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/sns/faqs/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/tools/</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AmazonVPC/latest/UserGuide/VPC_Route_Tables.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/IAM/latest/UserGuide/reference_policies_evaluation-logic.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStacks.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/general/latest/gr/aws_service_limits.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_BundleInstance.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/sns/latest/dg/SendMessageToHttp.html</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/AmazonS3/latest/dev/s3-access-control.html</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/autoscaling/</t>
+  </si>
+  <si>
+    <t>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html</t>
   </si>
 </sst>
 </file>
@@ -2124,7 +2124,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2143,65 +2143,65 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="str">
         <f>B1</f>
-        <v>https://aws.amazon.com/swf/faqs/</v>
+        <v>http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSSnapshots.html</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>CONCATENATE(A1,B1,C1,D1,E1)</f>
-        <v>&lt;a href="https://aws.amazon.com/swf/faqs/"&gt;https://aws.amazon.com/swf/faqs/&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSSnapshots.html"&gt;http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/EBSSnapshots.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="str">
         <f t="shared" ref="D2:D30" si="0">B2</f>
-        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/using-cfn-describing-stacks.html</v>
+        <v>https://aws.amazon.com/sns/faqs/</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f t="shared" ref="F2:F30" si="1">CONCATENATE(A2,B2,C2,D2,E2)</f>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/using-cfn-describing-stacks.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/using-cfn-describing-stacks.html&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/sns/faqs/"&gt;https://aws.amazon.com/sns/faqs/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html </v>
+        <v>https://aws.amazon.com/tools/</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html "&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html &lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/tools/"&gt;https://aws.amazon.com/tools/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2209,449 +2209,457 @@
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">https://aws.amazon.com/sns/faqs/ </v>
+        <v>http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://aws.amazon.com/sns/faqs/ "&gt;https://aws.amazon.com/sns/faqs/ &lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html"&gt;http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStackResources.html </v>
+        <v>http://docs.aws.amazon.com/AmazonVPC/latest/UserGuide/VPC_Route_Tables.html</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStackResources.html "&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStackResources.html &lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AmazonVPC/latest/UserGuide/VPC_Route_Tables.html"&gt;http://docs.aws.amazon.com/AmazonVPC/latest/UserGuide/VPC_Route_Tables.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> https://aws.amazon.com/dynamodb/faqs/</v>
+        <v>http://docs.aws.amazon.com/IAM/latest/UserGuide/reference_policies_evaluation-logic.html</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=" https://aws.amazon.com/dynamodb/faqs/"&gt; https://aws.amazon.com/dynamodb/faqs/&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/IAM/latest/UserGuide/reference_policies_evaluation-logic.html"&gt;http://docs.aws.amazon.com/IAM/latest/UserGuide/reference_policies_evaluation-logic.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/parameters-section-structure.html</v>
+        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStacks.html</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/parameters-section-structure.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/parameters-section-structure.html&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStacks.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/APIReference/API_ListStacks.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/aws-properties-ec2-instance.html</v>
+        <v>http://docs.aws.amazon.com/general/latest/gr/aws_service_limits.html</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/aws-properties-ec2-instance.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/aws-properties-ec2-instance.html&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/general/latest/gr/aws_service_limits.html"&gt;http://docs.aws.amazon.com/general/latest/gr/aws_service_limits.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">http://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html </v>
+        <v>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html "&gt;http://docs.aws.amazon.com/AmazonS3/latest/API/ErrorResponses.html &lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html"&gt;http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-register.html </v>
+        <v>http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_BundleInstance.html</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-register.html "&gt;http://docs.aws.amazon.com/sns/latest/dg/mobile-push-send-register.html &lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_BundleInstance.html"&gt;http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_BundleInstance.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>520</v>
-      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="2" t="str">
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html#limits-secondary-indexes</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html#limits-secondary-indexes"&gt;https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html#limits-secondary-indexes&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-getatt.html</v>
+        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-getatt.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-getatt.html&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html</v>
+        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html"&gt;http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_DescribeImages.html </v>
+        <v>https://aws.amazon.com/swf/faqs/</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_DescribeImages.html "&gt;http://docs.aws.amazon.com/AWSEC2/latest/APIReference/API_DescribeImages.html &lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/swf/faqs/"&gt;https://aws.amazon.com/swf/faqs/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>524</v>
-      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="str">
+      <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>https://aws.amazon.com/cloudformation/faqs/</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://aws.amazon.com/cloudformation/faqs/"&gt;https://aws.amazon.com/cloudformation/faqs/&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">http://docs.aws.amazon.com/AmazonS3/latest/dev/access-policy-language-overview.html </v>
+        <v>http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/access-policy-language-overview.html "&gt;http://docs.aws.amazon.com/AmazonS3/latest/dev/access-policy-language-overview.html &lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html"&gt;http://docs.aws.amazon.com/AWSCloudFormation/latest/UserGuide/intrinsic-function-reference-select.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">https://aws.amazon.com/blogs/developer/elasticache-as-an-asp-net-session-store/ </v>
+        <v>http://docs.aws.amazon.com/sns/latest/dg/SendMessageToHttp.html</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="https://aws.amazon.com/blogs/developer/elasticache-as-an-asp-net-session-store/ "&gt;https://aws.amazon.com/blogs/developer/elasticache-as-an-asp-net-session-store/ &lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="http://docs.aws.amazon.com/sns/latest/dg/SendMessageToHttp.html"&gt;http://docs.aws.amazon.com/sns/latest/dg/SendMessageToHttp.html&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/SecondaryIndexes.html</v>
+        <v>http://docs.aws.amazon.com/AmazonS3/latest/dev/s3-access-control.html</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F18" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/SecondaryIndexes.html"&gt;http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/SecondaryIndexes.html&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="http://docs.aws.amazon.com/AmazonS3/latest/dev/s3-access-control.html"&gt;http://docs.aws.amazon.com/AmazonS3/latest/dev/s3-access-control.html&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>511</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html"&gt;http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/ComponentsAMIs.html&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>510</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/swf/faqs/</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/swf/faqs/"&gt;https://aws.amazon.com/swf/faqs/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>512</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/dynamodb/faqs/</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/dynamodb/faqs/"&gt;https://aws.amazon.com/dynamodb/faqs/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>521</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F22" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html"&gt;http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/Limits.html&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>526</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/autoscaling/</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/autoscaling/"&gt;https://aws.amazon.com/autoscaling/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>527</v>
+      </c>
       <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F24" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html"&gt;http://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2776,25 +2784,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{C130B6E5-41F4-45EA-9BC1-FAF8CF17C674}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D2CEF5CD-C8A9-4AB4-AE22-B861B3435F22}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{89F6DD1E-DD3C-4E7F-A950-8F382AF52FE6}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{07716F62-E047-43FA-8D5A-59AC08F252F6}"/>
-    <hyperlink ref="B7" r:id="rId5" xr:uid="{5786EA90-4CE2-4C60-8A00-BB31F32CEC69}"/>
-    <hyperlink ref="B8" r:id="rId6" xr:uid="{934A8B7E-CCE2-432D-9C4D-3C7040ED02ED}"/>
-    <hyperlink ref="B9" r:id="rId7" xr:uid="{F0051B84-C21C-42DA-B4B2-5BCA4778D1D1}"/>
-    <hyperlink ref="B10" r:id="rId8" xr:uid="{319473A7-71E0-4DA3-9BAE-218051FBFE54}"/>
-    <hyperlink ref="B11" r:id="rId9" location="limits-secondary-indexes" xr:uid="{3FF1379B-D566-4052-9AD6-2DB90EF47A3D}"/>
-    <hyperlink ref="B12" r:id="rId10" xr:uid="{2776D543-5584-40CA-B894-43FD3AA54467}"/>
-    <hyperlink ref="B13" r:id="rId11" xr:uid="{CD175AB4-DC43-4380-995B-AEDAC2249F81}"/>
-    <hyperlink ref="B14" r:id="rId12" xr:uid="{6E182E47-59A3-4363-8B87-17B72A4C9125}"/>
-    <hyperlink ref="B15" r:id="rId13" xr:uid="{07ECEBBE-E293-445D-AEE1-BE565EB87C18}"/>
-    <hyperlink ref="B16" r:id="rId14" xr:uid="{9E6B17D7-02E4-41A9-A258-BD84DD2BAA89}"/>
-    <hyperlink ref="B17" r:id="rId15" xr:uid="{AF73AC59-B48D-465C-ABB0-2EB240F6B167}"/>
-    <hyperlink ref="B18" r:id="rId16" xr:uid="{092A8EA0-10AE-4378-81BF-6F1E232546B8}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1F30FF9D-70F6-4068-A09E-C5B931EA13D1}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{95E0B7F4-0331-4244-8631-D8AAB3E6BF2B}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{A8861BBB-4195-4F15-8E55-D35ED2195C09}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{FEE314B1-CABD-4078-9F8F-A12DA19F8C72}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{21985A55-4035-40C3-B9B5-44147F75520F}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{973D494F-1C38-4C73-BD0C-BEDAF6621E49}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{AE1578FD-BD8B-4E06-A0D9-85AC1D1AA323}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{6965B6F2-255B-4E34-9BA9-CF987FF8B131}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{5DAFE40E-3F0A-4EE6-971A-10680BD764D6}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{0F36E10F-E75C-4FC3-8BAB-0951235E46B6}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{F0D290DD-7D1C-47F1-B807-ADAA1D212AD8}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{0642E7E4-3CD0-4E6E-B3BB-5896302F1352}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{66AE58BF-F1AE-45BD-9C4A-4E6EA23155E7}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{EC5EC893-B4F5-4283-9081-156CE687523A}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{FB1FBA5C-9E82-4817-B8B2-864443B597F3}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{BD58DF8A-8E4B-45B6-9FF7-9A36D783824A}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{3D786A1F-EB04-42B4-87AF-619BC36343B0}"/>
+    <hyperlink ref="B21" r:id="rId18" xr:uid="{E8533553-AE48-43BC-AAAD-74CC04158C47}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{1C8BF399-F064-4648-8CEB-63FBFEE36C2E}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{37BD0D7B-3DA0-42BD-A867-3ECCE5FF54C0}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{856002B5-6E64-4009-A8DE-0B43B5044888}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
rt-3/4 (2) + extra formatting fix
</commit_message>
<xml_diff>
--- a/link-template.xlsx
+++ b/link-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\@AWS\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFA7443-2A8A-4152-8B7C-2CBB136E5984}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3F16C4-F44E-4A73-BD1C-7B141A7D6A11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="521">
   <si>
     <t>"&gt;</t>
   </si>
@@ -1615,10 +1615,34 @@
     <t>~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~~&lt;/br&gt;</t>
   </si>
   <si>
-    <t>https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.db.html</t>
-  </si>
-  <si>
-    <t>https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html</t>
+    <t>https://aws.amazon.com/blogs/database/choosing-the-right-dynamodb-partition-key/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ec2/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/ecs/faqs/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/codestar/features/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/blogs/mt/use-parameter-store-to-securely-access-secrets-and-config-data-in-aws-codedeploy/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/about-aws/whats-new/2017/07/amazon-cloudwatch-introduces-high-resolution-custom-metrics-and-alarms/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/dynamodb/dax/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/</t>
+  </si>
+  <si>
+    <t>https://aws.amazon.com/about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1737,7 +1761,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2079,14 +2102,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" style="4" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="90.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" style="5" customWidth="1"/>
     <col min="3" max="3" width="2.33203125" style="4" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="45.109375" style="4" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" style="4" hidden="1" customWidth="1"/>
@@ -2102,30 +2125,30 @@
         <v>510</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>511</v>
+      <c r="B2" s="5" t="s">
+        <v>512</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.db.html</v>
+        <v>https://aws.amazon.com/ec2/</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="str">
         <f>CONCATENATE(A2,B2,C2,D2,E2)</f>
-        <v>&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.db.html"&gt;https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.db.html&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/ec2/"&gt;https://aws.amazon.com/ec2/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G2" s="4" t="str">
         <f t="shared" ref="G2:G4" si="0">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(F2,"&gt;https://d0.awsstatic.com/","&gt;"),"&gt;https://aws.amazon.com/","&gt;"),"&gt;http://docs.aws.amazon.com/","&gt;"),"&gt;https://docs.aws.amazon.com/","&gt;"),"&gt;https://forums.aws.amazon.com/","&gt;"),".html&lt;/a&gt;&lt;/br&gt;","&lt;/a&gt;&lt;/br&gt;")</f>
-        <v>&lt;a href="https://docs.aws.amazon.com/elasticbeanstalk/latest/dg/using-features.managing.db.html"&gt;elasticbeanstalk/latest/dg/using-features.managing.db&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/ec2/"&gt;ec2/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2133,224 +2156,239 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="str">
         <f t="shared" ref="D3:D31" si="1">B3</f>
-        <v>https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html</v>
+        <v>https://aws.amazon.com/blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="str">
         <f t="shared" ref="F3:F31" si="2">CONCATENATE(A3,B3,C3,D3,E3)</f>
-        <v>&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html"&gt;https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/"&gt;https://aws.amazon.com/blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G3" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href="https://docs.aws.amazon.com/amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput.html"&gt;amazondynamodb/latest/developerguide/HowItWorks.ProvisionedThroughput&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/"&gt;blogs/big-data/preprocessing-data-in-amazon-kinesis-analytics-with-aws-lambda/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>511</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/blogs/database/choosing-the-right-dynamodb-partition-key/</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/blogs/database/choosing-the-right-dynamodb-partition-key/"&gt;https://aws.amazon.com/blogs/database/choosing-the-right-dynamodb-partition-key/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/blogs/database/choosing-the-right-dynamodb-partition-key/"&gt;blogs/database/choosing-the-right-dynamodb-partition-key/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>514</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/ecs/faqs/</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/ecs/faqs/"&gt;https://aws.amazon.com/ecs/faqs/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G5" s="4" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(F5,"&gt;https://d0.awsstatic.com/","&gt;"),"&gt;https://aws.amazon.com/","&gt;"),"&gt;http://docs.aws.amazon.com/","&gt;"),"&gt;https://docs.aws.amazon.com/","&gt;"),"&gt;https://forums.aws.amazon.com/","&gt;"),".html&lt;/a&gt;&lt;/br&gt;","&lt;/a&gt;&lt;/br&gt;")</f>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/ecs/faqs/"&gt;ecs/faqs/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>515</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/codestar/features/</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/codestar/features/"&gt;https://aws.amazon.com/codestar/features/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G6" s="4" t="str">
         <f t="shared" ref="G6:G31" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(F6,"&gt;https://d0.awsstatic.com/","&gt;"),"&gt;https://aws.amazon.com/","&gt;"),"&gt;http://docs.aws.amazon.com/","&gt;"),"&gt;https://docs.aws.amazon.com/","&gt;"),"&gt;https://forums.aws.amazon.com/","&gt;"),".html&lt;/a&gt;&lt;/br&gt;","&lt;/a&gt;&lt;/br&gt;")</f>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/codestar/features/"&gt;codestar/features/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>516</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/blogs/mt/use-parameter-store-to-securely-access-secrets-and-config-data-in-aws-codedeploy/</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/blogs/mt/use-parameter-store-to-securely-access-secrets-and-config-data-in-aws-codedeploy/"&gt;https://aws.amazon.com/blogs/mt/use-parameter-store-to-securely-access-secrets-and-config-data-in-aws-codedeploy/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G7" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/blogs/mt/use-parameter-store-to-securely-access-secrets-and-config-data-in-aws-codedeploy/"&gt;blogs/mt/use-parameter-store-to-securely-access-secrets-and-config-data-in-aws-codedeploy/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>517</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/about-aws/whats-new/2017/07/amazon-cloudwatch-introduces-high-resolution-custom-metrics-and-alarms/</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/about-aws/whats-new/2017/07/amazon-cloudwatch-introduces-high-resolution-custom-metrics-and-alarms/"&gt;https://aws.amazon.com/about-aws/whats-new/2017/07/amazon-cloudwatch-introduces-high-resolution-custom-metrics-and-alarms/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G8" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/about-aws/whats-new/2017/07/amazon-cloudwatch-introduces-high-resolution-custom-metrics-and-alarms/"&gt;about-aws/whats-new/2017/07/amazon-cloudwatch-introduces-high-resolution-custom-metrics-and-alarms/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>518</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/dynamodb/dax/</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/dynamodb/dax/"&gt;https://aws.amazon.com/dynamodb/dax/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G9" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/dynamodb/dax/"&gt;dynamodb/dax/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>519</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/"&gt;https://aws.amazon.com/blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G10" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>&lt;a href="https://aws.amazon.com/blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/"&gt;blogs/aws/new-amazon-ec2-feature-bring-your-own-keypair/&lt;/a&gt;&lt;/br&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>520</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>https://aws.amazon.com/about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/"&gt;https://aws.amazon.com/about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
       <c r="G11" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>&lt;a href=""&gt;0&lt;/a&gt;&lt;/br&gt;</v>
+        <v>&lt;a href="https://aws.amazon.com/about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/"&gt;about-aws/whats-new/2018/07/amazon-s3-announces-increased-request-rate-performance/&lt;/a&gt;&lt;/br&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="5"/>
       <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +2412,6 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="5"/>
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
@@ -2398,7 +2435,6 @@
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5"/>
       <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
@@ -2422,7 +2458,6 @@
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
@@ -2446,7 +2481,6 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="5"/>
       <c r="C16" s="3" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +2504,6 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="5"/>
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
@@ -2494,7 +2527,6 @@
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5"/>
       <c r="C18" s="3" t="s">
         <v>0</v>
       </c>
@@ -2518,7 +2550,6 @@
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="5"/>
       <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2542,7 +2573,6 @@
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="5"/>
       <c r="C20" s="3" t="s">
         <v>0</v>
       </c>
@@ -2566,7 +2596,6 @@
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="5"/>
       <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2619,6 @@
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="5"/>
       <c r="C22" s="3" t="s">
         <v>0</v>
       </c>
@@ -2614,7 +2642,6 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="5"/>
       <c r="C23" s="3" t="s">
         <v>0</v>
       </c>
@@ -2638,7 +2665,6 @@
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="5"/>
       <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
@@ -2662,7 +2688,6 @@
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="5"/>
       <c r="C25" s="3" t="s">
         <v>0</v>
       </c>
@@ -2686,7 +2711,6 @@
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="5"/>
       <c r="C26" s="3" t="s">
         <v>0</v>
       </c>
@@ -2710,7 +2734,6 @@
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="5"/>
       <c r="C27" s="3" t="s">
         <v>0</v>
       </c>
@@ -2734,7 +2757,6 @@
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="5"/>
       <c r="C28" s="3" t="s">
         <v>0</v>
       </c>
@@ -2758,7 +2780,6 @@
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="5"/>
       <c r="C29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2782,7 +2803,6 @@
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="5"/>
       <c r="C30" s="3" t="s">
         <v>0</v>
       </c>
@@ -2806,7 +2826,6 @@
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="2"/>
       <c r="C31" s="3" t="s">
         <v>0</v>
       </c>
@@ -2828,11 +2847,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F4D401E9-EDF2-407C-9112-2E7BF28A1B97}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{05BDC7C2-12AB-4610-8438-5AE1733399C7}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{169341F6-0A9A-4B2F-94C0-C2B10DDADB42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>